<commit_message>
third commit and working code
</commit_message>
<xml_diff>
--- a/data/api.xlsx
+++ b/data/api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Mans1611\University\Advanced Computer Programming\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7825A48E-B70E-45BB-BF5C-E3AA1A59D4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE4C889-0E6B-4DE2-8647-5C2C8E214486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2700" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5544" yWindow="3600" windowWidth="13824" windowHeight="7104" tabRatio="441" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="41" r:id="rId1"/>
@@ -792,12 +792,12 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="1" max="1" width="34.77734375" customWidth="1"/>
     <col min="2" max="2" width="45.5546875" customWidth="1"/>
     <col min="3" max="3" width="28.109375" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>

</xml_diff>